<commit_message>
minor changes to comments
</commit_message>
<xml_diff>
--- a/src/Tests/Tests.Daterpillar/data.xlsx
+++ b/src/Tests/Tests.Daterpillar/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Text_Formats" sheetId="1" r:id="rId1"/>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -835,7 +835,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
@@ -1025,7 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
* refactor test project * update assembly version
</commit_message>
<xml_diff>
--- a/src/Tests/Tests.Daterpillar/data.xlsx
+++ b/src/Tests/Tests.Daterpillar/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>TEXT</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>On_Device</t>
+  </si>
+  <si>
+    <t>BIT</t>
+  </si>
+  <si>
+    <t>VARBINARY(0)</t>
   </si>
 </sst>
 </file>
@@ -774,7 +780,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -782,7 +788,7 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -815,6 +821,9 @@
       <c r="D2" t="s">
         <v>54</v>
       </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -829,6 +838,9 @@
       <c r="D3" t="s">
         <v>55</v>
       </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -843,6 +855,9 @@
       <c r="D4" t="s">
         <v>69</v>
       </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -857,6 +872,9 @@
       <c r="D5" t="s">
         <v>0</v>
       </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -871,6 +889,9 @@
       <c r="D6" t="s">
         <v>63</v>
       </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -885,6 +906,9 @@
       <c r="D7" t="s">
         <v>56</v>
       </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -899,6 +923,9 @@
       <c r="D8" t="s">
         <v>62</v>
       </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -913,6 +940,9 @@
       <c r="D9" t="s">
         <v>56</v>
       </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -927,6 +957,9 @@
       <c r="D10" t="s">
         <v>56</v>
       </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -941,6 +974,9 @@
       <c r="D11" t="s">
         <v>57</v>
       </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -955,6 +991,9 @@
       <c r="D12" t="s">
         <v>58</v>
       </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -969,6 +1008,9 @@
       <c r="D13" t="s">
         <v>64</v>
       </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -983,6 +1025,9 @@
       <c r="D14" t="s">
         <v>59</v>
       </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -997,6 +1042,9 @@
       <c r="D15" t="s">
         <v>60</v>
       </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1009,6 +1057,9 @@
         <v>61</v>
       </c>
       <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add: type name resolver add: sql template update: namespace
</commit_message>
<xml_diff>
--- a/src/Tests/Tests.Daterpillar/data.xlsx
+++ b/src/Tests/Tests.Daterpillar/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Text_Formats" sheetId="1" r:id="rId1"/>
@@ -272,7 +272,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,7 +408,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -443,7 +443,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -620,7 +620,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -634,11 +634,11 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -783,12 +783,12 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -992,7 +992,7 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1080,15 +1080,15 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
implement and validate sql template
</commit_message>
<xml_diff>
--- a/src/Tests/Tests.Daterpillar/data.xlsx
+++ b/src/Tests/Tests.Daterpillar/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Text_Formats" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="84">
   <si>
     <t>TEXT</t>
   </si>
@@ -266,13 +266,19 @@
     <t>BIT</t>
   </si>
   <si>
-    <t>VARBINARY(0)</t>
+    <t>VARBINARY(MAX)</t>
+  </si>
+  <si>
+    <t>CHAR(MAX)</t>
+  </si>
+  <si>
+    <t>VARCHAR(MAX)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -620,7 +626,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -634,11 +640,11 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -780,15 +786,15 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -856,7 +862,7 @@
         <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -890,7 +896,7 @@
         <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1080,15 +1086,15 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>